<commit_message>
feat(reports): rename Citas resources to Informes  and create Citas module
-feat: Introduces a new feature.rename
-Citas to Reports: Main change description.
-create Citas module: Indicates the addition of the Citas module.
-add use case in controller: Specifies that the use case for Citas was
implemented in the controller
</commit_message>
<xml_diff>
--- a/temp/doctorchat_informe_medico.xlsx
+++ b/temp/doctorchat_informe_medico.xlsx
@@ -40,29 +40,21 @@
     <t>PRE INFORME MEDICO</t>
   </si>
   <si>
-    <t xml:space="preserve">El paciente reporta dolor de cabeza y mareo de dos días de duración. Recomienda consulta con neurólogo por posible origen neurológico. 
+    <t xml:space="preserve">El usuario reporta dolor de cabeza y mareos desde hace dos días. Se recomienda consultar con un neurólogo debido a la posible relación con problemas neurológicos. 
 </t>
   </si>
   <si>
     <t>RESUMEN DE SINTOMAS</t>
   </si>
   <si>
-    <t xml:space="preserve">El usuario experimenta dolor de cabeza y mareos desde hace dos días. 
+    <t xml:space="preserve">El usuario mencionó que tiene dolor de cabeza y mareos desde hace dos días. 
 </t>
   </si>
   <si>
     <t>RECOMENDACIÓN PARA EL ESPECIALISTA</t>
   </si>
   <si>
-    <t xml:space="preserve">Al llegar a la consulta, deberías preguntar al paciente qué otras molestias o síntomas experimenta además del dolor de cabeza y el mareo. Por ejemplo, podrías preguntar:
-* ¿Ha notado algún cambio en su visión?
-* ¿Tiene debilidad o entumecimiento en alguna parte del cuerpo?
-* ¿Ha tenido algún episodio de vómito o náuseas?
-* ¿Ha experimentado alguna pérdida de la consciencia o confusión?
-* ¿Ha tenido algún trauma en la cabeza recientemente?
-* ¿Tiene algún historial familiar de problemas neurológicos? 
-* ¿Está tomando algún medicamento o suplemento?
-Conocer más detalles sobre la experiencia del paciente te ayudará a realizar una evaluación más completa y precisa. 
+    <t xml:space="preserve">Al llegar a la consulta, sería bueno que le preguntes al paciente qué otras cosas del cuerpo le molestan o si siente algún otro síntoma. Esto te dará una visión más amplia del problema y te ayudará a determinar si el dolor de cabeza y el mareo son parte de algo más grande. 
 </t>
   </si>
   <si>

</xml_diff>